<commit_message>
Combine DeepFace & FaceNet for detection
</commit_message>
<xml_diff>
--- a/app/data/Caption.xlsx
+++ b/app/data/Caption.xlsx
@@ -9,6 +9,7 @@
     <sheet state="visible" name="Nam (Vui) " sheetId="4" r:id="rId6"/>
     <sheet state="visible" name="Nam (BTH)" sheetId="5" r:id="rId7"/>
     <sheet state="visible" name="Nữ (Đeo kính)" sheetId="6" r:id="rId8"/>
+    <sheet state="visible" name=" Nam (đeo kính)" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="850">
   <si>
     <t>caption</t>
   </si>
@@ -2094,10 +2095,6 @@
 Mà không nhắn cho em ??</t>
   </si>
   <si>
-    <t>Tấm thân này chỉ biết ăn no ngủ kỹ
-Đã bao giờ biết chửi con đũy nào đâu</t>
-  </si>
-  <si>
     <t>Anh ơi virus đầy đường
 Nơi an toàn nhát là giường của anh</t>
   </si>
@@ -2580,10 +2577,6 @@
 Yêu thì đừng thả haha nha mình</t>
   </si>
   <si>
-    <t>Như thằng ỉa đùn
-Anh yêu em vãi cut</t>
-  </si>
-  <si>
     <t xml:space="preserve">Em là vậy đó thích được thì thích 
 Thích không được thì yêu </t>
   </si>
@@ -2711,10 +2704,6 @@
 Tất cả thành vô nghĩa</t>
   </si>
   <si>
-    <t>Em chỉ cần rep inbox
-Anh với em sẽ rock in bed</t>
-  </si>
-  <si>
     <t>Lần đầu nhìn thấy anh
 Tưởng không sao
 Mà lao đao không tưởng</t>
@@ -2726,6 +2715,18 @@
   <si>
     <t>Sáng em nhớ tôi
 Thì tối em nhớ sang</t>
+  </si>
+  <si>
+    <t>Tấm thân này chỉ biết ăn no ngủ kỹ
+Đã bao giờ biết chửi con đũy nào đâu</t>
+  </si>
+  <si>
+    <t>Em chỉ cần rep inbox
+Anh với em sẽ rock in bed</t>
+  </si>
+  <si>
+    <t>Như thằng ỉa đùn
+Anh yêu em vãi cut</t>
   </si>
   <si>
     <t>Bạn đeo kính cũng đẹp, không đeo kính cũng đẹp. Bạn mặc áo dài đẹp, mặc áo ngắn cũng đẹp. Bạn đeo ba lô đẹp, không đeo ba lô cũng vẫn đẹp… Mọi thứ về bạn tôi đều thích. Nhất là khi bạn mỉm cười với mình</t>
@@ -3097,13 +3098,336 @@
   </si>
   <si>
     <t>Nhìn thấy cậu xong tớ chỉ muốn trở thành kết tủa Bari Sunfat trong trái tim cậu mà thôi!</t>
+  </si>
+  <si>
+    <t>Cảm lạnh có thể là do gió. Nhưng anh bị cảm nắng chắc chắn là do em</t>
+  </si>
+  <si>
+    <t>Thời tiết trái gió dở trời. Cần người trái giới dở trò</t>
+  </si>
+  <si>
+    <t>Đừng như Hà Lan và Ngạn. Vì anh không muốn chúng ta là bạn</t>
+  </si>
+  <si>
+    <t>Em xem anh đã đủ ngầu, để anh quên mối tình đầu hay chưa</t>
+  </si>
+  <si>
+    <t>Xuân kiếm lì xì, Hạ kiếm kem. Thu kiếm hoa sữa, Đông kiếm em</t>
+  </si>
+  <si>
+    <t>Đông này anh lạnh lẽo, nụ cười em là thứ ấm áp nhất anh có thể mặc</t>
+  </si>
+  <si>
+    <t>Điện thoại báo pin yếu. Tim báo Đông này thiếu em.</t>
+  </si>
+  <si>
+    <t>Gió đông về lạnh quá, nhưng không bằng sự băng giá trong tim.</t>
+  </si>
+  <si>
+    <t>Lạnh quá, chăn 37 độ ở đâu nhỉ?</t>
+  </si>
+  <si>
+    <t>Sống ảo thì anh có. Nhưng sống cùng ai đó thì anh chưa</t>
+  </si>
+  <si>
+    <t>Trời thu đẹp nhất về đêm. Đời anh đẹp nhất là thêm em vào</t>
+  </si>
+  <si>
+    <t>Đêm Hà Nội sương mù bao phủ, nhớ em nhiều anh có ngủ được đâu</t>
+  </si>
+  <si>
+    <t>Bình minh thì ở phía Đông, bình yên thì ở phía anh đây nè</t>
+  </si>
+  <si>
+    <t>Có những ngày mệt chẳng muốn làm gì cả, chỉ muốn làm người yêu em</t>
+  </si>
+  <si>
+    <t>Không mơ cổ tích hoang đường. Chỉ mơ giấc mộng đời thường có em.</t>
+  </si>
+  <si>
+    <t>Anh đã bị nhiễm một căn bệnh gọi là yêu, và anh tin rằng anh đã mắc nó từ em.</t>
+  </si>
+  <si>
+    <t>Anh có một siêu năng lực là nhắm mắt lại là có thể nhìn thấy em</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Em ơi kính anh dính một lớp gì này.
+Đó chính là lớp diu
+</t>
+  </si>
+  <si>
+    <t>Tính mời em đi ăn tối nhưng lại sợ thành bữa tối của em.</t>
+  </si>
+  <si>
+    <t>Em có biết cơ thể em được tạo thành 70% từ nước không? và anh cảm thấy rất khát ngay bây giờ.</t>
+  </si>
+  <si>
+    <t>Anh đoán tên em là Google. Bởi vì em đang có mọi thứ mà anh đang tìm kiếm</t>
+  </si>
+  <si>
+    <t>Anh nghĩ điện thoại của anh gặp vấn đề rồi, nó chưa có số điện thoại của em.</t>
+  </si>
+  <si>
+    <t>Hà Nội không thể vì hoàng hôn mà trở nên rực rỡ. Nhưng anh có thể vì em mà trở nên yêu đời.</t>
+  </si>
+  <si>
+    <t>Đắc tội hôn đôi má em. Mong má em khoan hồng</t>
+  </si>
+  <si>
+    <t>Ô tô đã có chỗ đỗ. Còn anh thì đã đỗ trong tim em.</t>
+  </si>
+  <si>
+    <t>Anh không phải là cái lò vi sóng, nhưng anh đủ sức hâm nóng trái tim em.</t>
+  </si>
+  <si>
+    <t>Yêu em anh ngửa mặt lên trời. Vì em là cả bầu trời của anh.</t>
+  </si>
+  <si>
+    <t>Có thể những lời anh nói không phải lời đường mật, nhưng những điều anh dành cho em sẽ chân thật và ngọt ngào nhất.</t>
+  </si>
+  <si>
+    <t>Bao năm phê đá phê cần, không bằng một phút ngồi gần bên em.</t>
+  </si>
+  <si>
+    <t>Có một đốm lửa nhỏ. Thắp lên hạnh phúc to. Em đã có ai ngỏ. Hay là để anh lo</t>
+  </si>
+  <si>
+    <t>Đen Vâu muốn về quê trồng rau và nuôi cá, còn anh muốn về hỏi ba má cướiem.</t>
+  </si>
+  <si>
+    <t>Em có thể gửi cho anh một tấm hình của em không, bạn bè anh không tin thiên thần có thật</t>
+  </si>
+  <si>
+    <t>Chim thường yêu trời, con nít thường yêu kem. Anh thì rất yêu đời, và cũng rất yêu em</t>
+  </si>
+  <si>
+    <t>Anh đang muốn thứ gì đó ngọt ngào, cho anh nếm thử đôi môi của em được không.</t>
+  </si>
+  <si>
+    <t>Anh chỉ muốn ở bên em hai lần, đó là bây giờ và mãi mãi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiếu 500 nghìn là anh tròn một củ
+Thiếu em nữa là anh đủ một đôi.
+</t>
+  </si>
+  <si>
+    <t>Nếu ngoại hình có thể giết người thì em là một kẻ sát nhân ngọt ngào.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bao nhiêu cân thính cho vừa
+Bao nhiêu cân bả mới lừa được em.
+</t>
+  </si>
+  <si>
+    <t>Hình như anh quên mất cách ôm rồi, em có thể chỉ cho anh được không?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anh có một siêu năng lượng
+Đó là siêu thích em
+</t>
+  </si>
+  <si>
+    <t>Anh đang cố hết sức để ngủ, nhưng anh không thể ngừng nghĩ về em.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anh bận tất cả mọi điều
+Nhưng vẫn luôn rảnh để nhớ đến em.
+</t>
+  </si>
+  <si>
+    <t>Nếu em đang bị tổn thương, hãy để anh băng bó vết thương của em bằng cái ôm này.</t>
+  </si>
+  <si>
+    <t>Nếu anh hôn em và em không thích nó, em có thể trả lại anh nụ hôn này.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Người ta dính phốt ngoại tình
+Còn tôi dính phốt một mình lâu năm.
+</t>
+  </si>
+  <si>
+    <t>Nghe đây!, em đã bị bắt vì tội quá xinh đẹp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trái Đất quay quanh Mặt Trời
+Còn em thì quay mãi trong tâm trí anh.
+</t>
+  </si>
+  <si>
+    <t>Nếu em đứng trước gương và cầm 11 bông hồng, em sẽ thấy có một bông thứ 12 đẹp nhất.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đôi khi anh yêu một thành phố
+Không phải vì nó có gì, mà vì nó có em.
+</t>
+  </si>
+  <si>
+    <t>Nếu trái tim em là một nhà tù, anh nguyện bị kết án chung thân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lồng thì để anh nhốt chim
+Con em anh nhốt ở trong tim nè.
+</t>
+  </si>
+  <si>
+    <t>Nếu cái bóng của em là thứ đẹp thứ 2 trên thế giới này, thì điều gì sẽ đẹp nhất?</t>
+  </si>
+  <si>
+    <t>Anh đang gặp một vấn đề nghiêm trọng, đó là không thể ngừng nghĩ về em.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vector chỉ có một chiều
+Còn anh dân chuyên toán chỉ yêu 1 người.
+</t>
+  </si>
+  <si>
+    <t>Nếu những hạt mưa là những nụ hôn, anh sẽ gửi cho em một cơn mưa rào.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Em có tin vào duyên số không
+Nếu không thì em đưa số điện thoại đây.
+</t>
+  </si>
+  <si>
+    <t>Thiếu ăn, chim tìm con sâu. Thiếu em, anh sầu con tim.</t>
+  </si>
+  <si>
+    <t>Tại sao anh vẫn sợ mất em, ngay cả khi em không thuộc về anh?</t>
+  </si>
+  <si>
+    <t>Anh đã nhìn em từ phía sau, đúng là không phải thiên thần nào cũng có cánh.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngày em đến, em dạy anh các yêu thương trọn vẹn một người.
+Ngày em đi, em chưa dạy anh cách quên đi một người anh từng trọn vẹn yêu thương.
+</t>
+  </si>
+  <si>
+    <t>Có phải mẹ em đang tìm con rể?</t>
+  </si>
+  <si>
+    <t>Em có tấm bản đồ nào không, anh bị lạc trong mắt em rồi.</t>
+  </si>
+  <si>
+    <t>Như thế này liệu đã đủ tiêu chuẩn để làm bạn trai em chưa?</t>
+  </si>
+  <si>
+    <t>Trời mưa to và cây thì đang đổ, sao em còn chưa đổ anh.</t>
+  </si>
+  <si>
+    <t>Đến đôi dép còn có đôi, mà sao mình vẫn lẻ chiếc</t>
+  </si>
+  <si>
+    <t>Có lẽ anh không phải là một người đàn ông hoàn hảo, nhưng đủ tiêu chuẩn để làm bạn trai em</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trăng kia ai vẽ mà tròn
+Lòng anh ai trộm mà hoài nhớ thương
+</t>
+  </si>
+  <si>
+    <t>Anh biết có rất nhiều cách khiến người ta cảm thấy hạnh phúc, nhưng với anh cách nhanh nhất là được ở bên em.</t>
+  </si>
+  <si>
+    <t>Nếu không đúng là người mình cần, thì cho dù bên cạnh có bao nhiêu người chăng nữa, cũng vẫn thấy cô đơn</t>
+  </si>
+  <si>
+    <t>Anh có thể uống cà phê không đường, vì ở cạnh em, anh cảm thấy đủ ngọt ngào rồi.</t>
+  </si>
+  <si>
+    <t>Kiểm tra giới tính nhé mọi người! Ai giới tính NỮ thì ấn LIKE tay trái, ai giới tính NAM thì ấn LIKE tay phải! Còn giới tính THỨ BA thì ấn nút LIKE 3 lần nha</t>
+  </si>
+  <si>
+    <t>Chỉ cần em nói YÊU, anh sẽ bám theo em suốt đời</t>
+  </si>
+  <si>
+    <t>Anh trông em rất là quen. Trông em rất giống người yêu tương lai của anh đấy</t>
+  </si>
+  <si>
+    <t>Cuộc đời này chắc chắn không như ý em muốn, vậy anh sẽ như ý em muốn.</t>
+  </si>
+  <si>
+    <t>Anh không muốn say bia hay say rượu nữa. Anh chỉ muốn say ánh mắt của em</t>
+  </si>
+  <si>
+    <t>Câu thả thính là anh copy, nhưng tình cảm anh dành cho em là thật.</t>
+  </si>
+  <si>
+    <t>Đẹp nhất không phải là ngày mưa mà là ngày cùng em nhận giấy khen Gia đình văn hóa</t>
+  </si>
+  <si>
+    <t>Ngoài kia đám cưới linh đình. Bao giờ thì đến lượt mình em ơi.</t>
+  </si>
+  <si>
+    <t>Tiết kiệm nước là chính sách quốc gia, thế nên em đừng tắm một mình nữa</t>
+  </si>
+  <si>
+    <t>Tay anh đây ấm lắm, em muốn nắm thử không</t>
+  </si>
+  <si>
+    <t>Em không phải kiểu người mà anh thích. Nhưng em là người anh thích.</t>
+  </si>
+  <si>
+    <t>Nếu anh là cảnh sát giao thông thì anh sẽ cấm em đi ngoài đường, bởi vì em sẽ khiến cho các chàng trai gây tai nạn.</t>
+  </si>
+  <si>
+    <t>Người khác thích em sẽ đưa em hoa, đưa em quà. Nhưng anh chỉ muốn đưa em về nhà</t>
+  </si>
+  <si>
+    <t>Mọi người đều yêu cái đẹp, nên anh yêu em.</t>
+  </si>
+  <si>
+    <t>Anh đã xem hết “Mười vạn câu hỏi vì sao” những vẫn chẳng giải thích được vì sao anh thích em</t>
+  </si>
+  <si>
+    <t>Bố em có phải là một thợ kim hoàn không? Sao em giống viên kim cương vậy?</t>
+  </si>
+  <si>
+    <t>Mình cũng đẹp trai đấy chứ nhỉ, vậy mà bao nhiêu năm rồi chưa một mảnh tình vắt vai là sao vậy?</t>
+  </si>
+  <si>
+    <t>Với thế giới thì em chỉ là một người. Còn với anh, em là cả thế giới.</t>
+  </si>
+  <si>
+    <t>Em có muốn làm Mặt Trời duy nhất của anh không?</t>
+  </si>
+  <si>
+    <t>Này em ơi, mẹ anh đang gọi con dâu kìa.</t>
+  </si>
+  <si>
+    <t>Chỉ cần em yêu anh thôi, còn cả thế giới cứ để anh lo.</t>
+  </si>
+  <si>
+    <t>Giờ nếu có cô gái nào nguyện bên anh, anh sẽ khiến cô ấy hạnh phúc mãi về sau.</t>
+  </si>
+  <si>
+    <t>Đố em một con gấu bắc cực nặng bao nhiêu kg? Anh cũng không biết nhưng anh biết con gấu bắc cực đủ nặng để phá vỡ tảng băng giữa chúng ta.</t>
+  </si>
+  <si>
+    <t>Anh đứng ở đây từ chiều mà chưa thấy cô gái nào dễ thương như em đi qua đây.</t>
+  </si>
+  <si>
+    <t>Mọi người cần ăn một ngày 3 bữa để tồn tại. Còn anh thì chỉ cần ăn em</t>
+  </si>
+  <si>
+    <t>Muối tan khi ngoáy lên trong nuớc còn anh thấy em  là tự tan rồi…</t>
+  </si>
+  <si>
+    <t>Người ta thích đi vòng quanh thế giới. Còn anh chỉ thích đi vòng quanh em</t>
+  </si>
+  <si>
+    <t>Anh đeo kính là để chống lại tia nắng tỏa ra từ em đấy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dù mắt anh không tỏ, nhưng anh rõ lòng mình thích em </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -3113,13 +3437,40 @@
     <font>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF222222"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3128,7 +3479,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3143,6 +3494,25 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3176,6 +3546,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -7190,16 +7564,13 @@
       </c>
     </row>
     <row r="501">
-      <c r="A501" s="1" t="s">
-        <v>500</v>
-      </c>
       <c r="B501" s="1">
         <v>513.0</v>
       </c>
     </row>
     <row r="502">
       <c r="A502" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B502" s="1">
         <v>514.0</v>
@@ -7207,7 +7578,7 @@
     </row>
     <row r="503">
       <c r="A503" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B503" s="1">
         <v>515.0</v>
@@ -7215,7 +7586,7 @@
     </row>
     <row r="504">
       <c r="A504" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B504" s="1">
         <v>516.0</v>
@@ -7223,7 +7594,7 @@
     </row>
     <row r="505">
       <c r="A505" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B505" s="1">
         <v>518.0</v>
@@ -7231,7 +7602,7 @@
     </row>
     <row r="506">
       <c r="A506" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B506" s="1">
         <v>519.0</v>
@@ -7239,7 +7610,7 @@
     </row>
     <row r="507">
       <c r="A507" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B507" s="1">
         <v>520.0</v>
@@ -7247,7 +7618,7 @@
     </row>
     <row r="508">
       <c r="A508" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B508" s="1">
         <v>521.0</v>
@@ -7255,7 +7626,7 @@
     </row>
     <row r="509">
       <c r="A509" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B509" s="1">
         <v>522.0</v>
@@ -7263,7 +7634,7 @@
     </row>
     <row r="510">
       <c r="A510" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B510" s="1">
         <v>523.0</v>
@@ -7271,7 +7642,7 @@
     </row>
     <row r="511">
       <c r="A511" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B511" s="1">
         <v>524.0</v>
@@ -7279,7 +7650,7 @@
     </row>
     <row r="512">
       <c r="A512" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B512" s="1">
         <v>525.0</v>
@@ -7287,7 +7658,7 @@
     </row>
     <row r="513">
       <c r="A513" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B513" s="1">
         <v>526.0</v>
@@ -7295,7 +7666,7 @@
     </row>
     <row r="514">
       <c r="A514" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B514" s="1">
         <v>527.0</v>
@@ -7303,7 +7674,7 @@
     </row>
     <row r="515">
       <c r="A515" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B515" s="1">
         <v>528.0</v>
@@ -7311,7 +7682,7 @@
     </row>
     <row r="516">
       <c r="A516" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B516" s="1">
         <v>529.0</v>
@@ -7319,7 +7690,7 @@
     </row>
     <row r="517">
       <c r="A517" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B517" s="1">
         <v>530.0</v>
@@ -7327,7 +7698,7 @@
     </row>
     <row r="518">
       <c r="A518" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B518" s="1">
         <v>531.0</v>
@@ -7335,7 +7706,7 @@
     </row>
     <row r="519">
       <c r="A519" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B519" s="1">
         <v>532.0</v>
@@ -7343,7 +7714,7 @@
     </row>
     <row r="520">
       <c r="A520" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B520" s="1">
         <v>533.0</v>
@@ -7351,7 +7722,7 @@
     </row>
     <row r="521">
       <c r="A521" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B521" s="1">
         <v>534.0</v>
@@ -7359,7 +7730,7 @@
     </row>
     <row r="522">
       <c r="A522" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B522" s="1">
         <v>535.0</v>
@@ -7367,7 +7738,7 @@
     </row>
     <row r="523">
       <c r="A523" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B523" s="1">
         <v>536.0</v>
@@ -7375,7 +7746,7 @@
     </row>
     <row r="524">
       <c r="A524" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B524" s="1">
         <v>537.0</v>
@@ -7383,7 +7754,7 @@
     </row>
     <row r="525">
       <c r="A525" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B525" s="1">
         <v>538.0</v>
@@ -7391,7 +7762,7 @@
     </row>
     <row r="526">
       <c r="A526" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B526" s="1">
         <v>539.0</v>
@@ -7399,7 +7770,7 @@
     </row>
     <row r="527">
       <c r="A527" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B527" s="1">
         <v>540.0</v>
@@ -7407,7 +7778,7 @@
     </row>
     <row r="528">
       <c r="A528" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B528" s="1">
         <v>541.0</v>
@@ -7415,7 +7786,7 @@
     </row>
     <row r="529">
       <c r="A529" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B529" s="1">
         <v>542.0</v>
@@ -7423,7 +7794,7 @@
     </row>
     <row r="530">
       <c r="A530" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B530" s="1">
         <v>543.0</v>
@@ -7431,7 +7802,7 @@
     </row>
     <row r="531">
       <c r="A531" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B531" s="1">
         <v>544.0</v>
@@ -7439,7 +7810,7 @@
     </row>
     <row r="532">
       <c r="A532" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B532" s="1">
         <v>545.0</v>
@@ -7447,7 +7818,7 @@
     </row>
     <row r="533">
       <c r="A533" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B533" s="1">
         <v>546.0</v>
@@ -7455,7 +7826,7 @@
     </row>
     <row r="534">
       <c r="A534" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B534" s="1">
         <v>547.0</v>
@@ -7463,7 +7834,7 @@
     </row>
     <row r="535">
       <c r="A535" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B535" s="1">
         <v>548.0</v>
@@ -7471,7 +7842,7 @@
     </row>
     <row r="536">
       <c r="A536" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B536" s="1">
         <v>549.0</v>
@@ -7479,7 +7850,7 @@
     </row>
     <row r="537">
       <c r="A537" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B537" s="1">
         <v>550.0</v>
@@ -7487,7 +7858,7 @@
     </row>
     <row r="538">
       <c r="A538" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B538" s="1">
         <v>551.0</v>
@@ -7495,7 +7866,7 @@
     </row>
     <row r="539">
       <c r="A539" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B539" s="1">
         <v>552.0</v>
@@ -7503,7 +7874,7 @@
     </row>
     <row r="540">
       <c r="A540" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B540" s="1">
         <v>553.0</v>
@@ -7511,7 +7882,7 @@
     </row>
     <row r="541">
       <c r="A541" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B541" s="1">
         <v>554.0</v>
@@ -7519,7 +7890,7 @@
     </row>
     <row r="542">
       <c r="A542" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B542" s="1">
         <v>555.0</v>
@@ -7527,7 +7898,7 @@
     </row>
     <row r="543">
       <c r="A543" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B543" s="1">
         <v>556.0</v>
@@ -7535,7 +7906,7 @@
     </row>
     <row r="544">
       <c r="A544" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B544" s="1">
         <v>557.0</v>
@@ -7543,7 +7914,7 @@
     </row>
     <row r="545">
       <c r="A545" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B545" s="1">
         <v>558.0</v>
@@ -7551,7 +7922,7 @@
     </row>
     <row r="546">
       <c r="A546" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B546" s="1">
         <v>559.0</v>
@@ -7559,7 +7930,7 @@
     </row>
     <row r="547">
       <c r="A547" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B547" s="1">
         <v>560.0</v>
@@ -7567,7 +7938,7 @@
     </row>
     <row r="548">
       <c r="A548" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B548" s="1">
         <v>561.0</v>
@@ -7575,7 +7946,7 @@
     </row>
     <row r="549">
       <c r="A549" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B549" s="1">
         <v>562.0</v>
@@ -7583,7 +7954,7 @@
     </row>
     <row r="550">
       <c r="A550" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B550" s="1">
         <v>563.0</v>
@@ -7591,7 +7962,7 @@
     </row>
     <row r="551">
       <c r="A551" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B551" s="1">
         <v>564.0</v>
@@ -7599,7 +7970,7 @@
     </row>
     <row r="552">
       <c r="A552" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B552" s="1">
         <v>565.0</v>
@@ -7607,7 +7978,7 @@
     </row>
     <row r="553">
       <c r="A553" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B553" s="1">
         <v>566.0</v>
@@ -7615,7 +7986,7 @@
     </row>
     <row r="554">
       <c r="A554" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B554" s="1">
         <v>567.0</v>
@@ -7623,7 +7994,7 @@
     </row>
     <row r="555">
       <c r="A555" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B555" s="1">
         <v>568.0</v>
@@ -7631,7 +8002,7 @@
     </row>
     <row r="556">
       <c r="A556" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B556" s="1">
         <v>569.0</v>
@@ -7639,7 +8010,7 @@
     </row>
     <row r="557">
       <c r="A557" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B557" s="1">
         <v>570.0</v>
@@ -7647,7 +8018,7 @@
     </row>
     <row r="558">
       <c r="A558" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B558" s="1">
         <v>571.0</v>
@@ -7655,7 +8026,7 @@
     </row>
     <row r="559">
       <c r="A559" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B559" s="1">
         <v>572.0</v>
@@ -7663,7 +8034,7 @@
     </row>
     <row r="560">
       <c r="A560" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B560" s="1">
         <v>573.0</v>
@@ -7671,7 +8042,7 @@
     </row>
     <row r="561">
       <c r="A561" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B561" s="1">
         <v>574.0</v>
@@ -7679,7 +8050,7 @@
     </row>
     <row r="562">
       <c r="A562" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B562" s="1">
         <v>575.0</v>
@@ -7687,7 +8058,7 @@
     </row>
     <row r="563">
       <c r="A563" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B563" s="1">
         <v>576.0</v>
@@ -7695,7 +8066,7 @@
     </row>
     <row r="564">
       <c r="A564" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B564" s="1">
         <v>577.0</v>
@@ -7703,7 +8074,7 @@
     </row>
     <row r="565">
       <c r="A565" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B565" s="1">
         <v>578.0</v>
@@ -7711,7 +8082,7 @@
     </row>
     <row r="566">
       <c r="A566" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B566" s="1">
         <v>579.0</v>
@@ -7719,7 +8090,7 @@
     </row>
     <row r="567">
       <c r="A567" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B567" s="1">
         <v>580.0</v>
@@ -7727,7 +8098,7 @@
     </row>
     <row r="568">
       <c r="A568" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B568" s="1">
         <v>581.0</v>
@@ -7735,7 +8106,7 @@
     </row>
     <row r="569">
       <c r="A569" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B569" s="1">
         <v>582.0</v>
@@ -7743,7 +8114,7 @@
     </row>
     <row r="570">
       <c r="A570" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B570" s="1">
         <v>583.0</v>
@@ -7751,7 +8122,7 @@
     </row>
     <row r="571">
       <c r="A571" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B571" s="1">
         <v>584.0</v>
@@ -7759,7 +8130,7 @@
     </row>
     <row r="572">
       <c r="A572" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B572" s="1">
         <v>585.0</v>
@@ -7767,7 +8138,7 @@
     </row>
     <row r="573">
       <c r="A573" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B573" s="1">
         <v>586.0</v>
@@ -7775,7 +8146,7 @@
     </row>
     <row r="574">
       <c r="A574" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B574" s="1">
         <v>587.0</v>
@@ -7783,7 +8154,7 @@
     </row>
     <row r="575">
       <c r="A575" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B575" s="1">
         <v>588.0</v>
@@ -7791,7 +8162,7 @@
     </row>
     <row r="576">
       <c r="A576" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B576" s="1">
         <v>589.0</v>
@@ -7799,7 +8170,7 @@
     </row>
     <row r="577">
       <c r="A577" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B577" s="1">
         <v>590.0</v>
@@ -7807,7 +8178,7 @@
     </row>
     <row r="578">
       <c r="A578" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B578" s="1">
         <v>591.0</v>
@@ -7815,7 +8186,7 @@
     </row>
     <row r="579">
       <c r="A579" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B579" s="1">
         <v>592.0</v>
@@ -7823,7 +8194,7 @@
     </row>
     <row r="580">
       <c r="A580" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B580" s="1">
         <v>593.0</v>
@@ -7831,7 +8202,7 @@
     </row>
     <row r="581">
       <c r="A581" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B581" s="1">
         <v>594.0</v>
@@ -7839,7 +8210,7 @@
     </row>
     <row r="582">
       <c r="A582" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B582" s="1">
         <v>595.0</v>
@@ -7847,7 +8218,7 @@
     </row>
     <row r="583">
       <c r="A583" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B583" s="1">
         <v>596.0</v>
@@ -7855,7 +8226,7 @@
     </row>
     <row r="584">
       <c r="A584" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B584" s="1">
         <v>597.0</v>
@@ -7863,7 +8234,7 @@
     </row>
     <row r="585">
       <c r="A585" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B585" s="1">
         <v>598.0</v>
@@ -7871,7 +8242,7 @@
     </row>
     <row r="586">
       <c r="A586" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B586" s="1">
         <v>599.0</v>
@@ -7879,7 +8250,7 @@
     </row>
     <row r="587">
       <c r="A587" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B587" s="1">
         <v>600.0</v>
@@ -7887,7 +8258,7 @@
     </row>
     <row r="588">
       <c r="A588" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B588" s="1">
         <v>601.0</v>
@@ -7895,7 +8266,7 @@
     </row>
     <row r="589">
       <c r="A589" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B589" s="1">
         <v>602.0</v>
@@ -7903,7 +8274,7 @@
     </row>
     <row r="590">
       <c r="A590" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B590" s="1">
         <v>603.0</v>
@@ -7911,7 +8282,7 @@
     </row>
     <row r="591">
       <c r="A591" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B591" s="1">
         <v>604.0</v>
@@ -7919,7 +8290,7 @@
     </row>
     <row r="592">
       <c r="A592" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B592" s="1">
         <v>605.0</v>
@@ -7927,7 +8298,7 @@
     </row>
     <row r="593">
       <c r="A593" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B593" s="1">
         <v>606.0</v>
@@ -7935,7 +8306,7 @@
     </row>
     <row r="594">
       <c r="A594" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B594" s="1">
         <v>607.0</v>
@@ -7943,7 +8314,7 @@
     </row>
     <row r="595">
       <c r="A595" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B595" s="1">
         <v>608.0</v>
@@ -7951,7 +8322,7 @@
     </row>
     <row r="596">
       <c r="A596" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B596" s="1">
         <v>609.0</v>
@@ -7959,7 +8330,7 @@
     </row>
     <row r="597">
       <c r="A597" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B597" s="1">
         <v>610.0</v>
@@ -7967,7 +8338,7 @@
     </row>
     <row r="598">
       <c r="A598" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B598" s="1">
         <v>611.0</v>
@@ -7975,7 +8346,7 @@
     </row>
     <row r="599">
       <c r="A599" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B599" s="1">
         <v>612.0</v>
@@ -7983,7 +8354,7 @@
     </row>
     <row r="600">
       <c r="A600" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B600" s="1">
         <v>613.0</v>
@@ -7991,7 +8362,7 @@
     </row>
     <row r="601">
       <c r="A601" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B601" s="1">
         <v>614.0</v>
@@ -7999,7 +8370,7 @@
     </row>
     <row r="602">
       <c r="A602" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B602" s="1">
         <v>615.0</v>
@@ -8007,7 +8378,7 @@
     </row>
     <row r="603">
       <c r="A603" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B603" s="1">
         <v>616.0</v>
@@ -8015,7 +8386,7 @@
     </row>
     <row r="604">
       <c r="A604" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B604" s="1">
         <v>617.0</v>
@@ -8023,7 +8394,7 @@
     </row>
     <row r="605">
       <c r="A605" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B605" s="1">
         <v>618.0</v>
@@ -8031,7 +8402,7 @@
     </row>
     <row r="606">
       <c r="A606" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B606" s="1">
         <v>619.0</v>
@@ -8039,7 +8410,7 @@
     </row>
     <row r="607">
       <c r="A607" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B607" s="1">
         <v>620.0</v>
@@ -8047,7 +8418,7 @@
     </row>
     <row r="608">
       <c r="A608" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B608" s="1">
         <v>621.0</v>
@@ -8055,7 +8426,7 @@
     </row>
     <row r="609">
       <c r="A609" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B609" s="1">
         <v>622.0</v>
@@ -8063,7 +8434,7 @@
     </row>
     <row r="610">
       <c r="A610" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B610" s="1">
         <v>623.0</v>
@@ -8071,7 +8442,7 @@
     </row>
     <row r="611">
       <c r="A611" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B611" s="1">
         <v>624.0</v>
@@ -8079,7 +8450,7 @@
     </row>
     <row r="612">
       <c r="A612" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B612" s="1">
         <v>625.0</v>
@@ -8087,7 +8458,7 @@
     </row>
     <row r="613">
       <c r="A613" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B613" s="1">
         <v>626.0</v>
@@ -8095,7 +8466,7 @@
     </row>
     <row r="614">
       <c r="A614" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B614" s="1">
         <v>627.0</v>
@@ -8103,7 +8474,7 @@
     </row>
     <row r="615">
       <c r="A615" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B615" s="1">
         <v>628.0</v>
@@ -8111,23 +8482,15 @@
     </row>
     <row r="616">
       <c r="A616" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B616" s="1">
         <v>629.0</v>
       </c>
     </row>
-    <row r="617">
-      <c r="A617" s="1" t="s">
-        <v>616</v>
-      </c>
-      <c r="B617" s="1">
-        <v>630.0</v>
-      </c>
-    </row>
     <row r="618">
       <c r="A618" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B618" s="1">
         <v>631.0</v>
@@ -8135,7 +8498,7 @@
     </row>
     <row r="619">
       <c r="A619" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B619" s="1">
         <v>632.0</v>
@@ -8143,7 +8506,7 @@
     </row>
     <row r="620">
       <c r="A620" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B620" s="1">
         <v>633.0</v>
@@ -8151,7 +8514,7 @@
     </row>
     <row r="621">
       <c r="A621" s="1" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B621" s="1">
         <v>634.0</v>
@@ -8159,7 +8522,7 @@
     </row>
     <row r="622">
       <c r="A622" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B622" s="1">
         <v>635.0</v>
@@ -8167,7 +8530,7 @@
     </row>
     <row r="623">
       <c r="A623" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B623" s="1">
         <v>636.0</v>
@@ -8175,7 +8538,7 @@
     </row>
     <row r="624">
       <c r="A624" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B624" s="1">
         <v>637.0</v>
@@ -8183,7 +8546,7 @@
     </row>
     <row r="625">
       <c r="A625" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B625" s="1">
         <v>638.0</v>
@@ -8191,7 +8554,7 @@
     </row>
     <row r="626">
       <c r="A626" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B626" s="1">
         <v>639.0</v>
@@ -8199,7 +8562,7 @@
     </row>
     <row r="627">
       <c r="A627" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B627" s="1">
         <v>640.0</v>
@@ -8207,7 +8570,7 @@
     </row>
     <row r="628">
       <c r="A628" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B628" s="1">
         <v>641.0</v>
@@ -8215,7 +8578,7 @@
     </row>
     <row r="629">
       <c r="A629" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B629" s="1">
         <v>642.0</v>
@@ -8223,7 +8586,7 @@
     </row>
     <row r="630">
       <c r="A630" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B630" s="1">
         <v>643.0</v>
@@ -8231,7 +8594,7 @@
     </row>
     <row r="631">
       <c r="A631" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B631" s="1">
         <v>644.0</v>
@@ -8239,7 +8602,7 @@
     </row>
     <row r="632">
       <c r="A632" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B632" s="1">
         <v>645.0</v>
@@ -8247,7 +8610,7 @@
     </row>
     <row r="633">
       <c r="A633" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B633" s="1">
         <v>646.0</v>
@@ -8255,7 +8618,7 @@
     </row>
     <row r="634">
       <c r="A634" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B634" s="1">
         <v>647.0</v>
@@ -8263,7 +8626,7 @@
     </row>
     <row r="635">
       <c r="A635" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B635" s="1">
         <v>648.0</v>
@@ -8271,7 +8634,7 @@
     </row>
     <row r="636">
       <c r="A636" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B636" s="1">
         <v>649.0</v>
@@ -8279,7 +8642,7 @@
     </row>
     <row r="637">
       <c r="A637" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B637" s="1">
         <v>650.0</v>
@@ -8287,7 +8650,7 @@
     </row>
     <row r="638">
       <c r="A638" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B638" s="1">
         <v>651.0</v>
@@ -8295,7 +8658,7 @@
     </row>
     <row r="639">
       <c r="A639" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B639" s="1">
         <v>652.0</v>
@@ -8303,7 +8666,7 @@
     </row>
     <row r="640">
       <c r="A640" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B640" s="1">
         <v>653.0</v>
@@ -8311,7 +8674,7 @@
     </row>
     <row r="641">
       <c r="A641" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B641" s="1">
         <v>654.0</v>
@@ -8319,7 +8682,7 @@
     </row>
     <row r="642">
       <c r="A642" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B642" s="1">
         <v>655.0</v>
@@ -8327,7 +8690,7 @@
     </row>
     <row r="643">
       <c r="A643" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B643" s="1">
         <v>656.0</v>
@@ -8335,7 +8698,7 @@
     </row>
     <row r="644">
       <c r="A644" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B644" s="1">
         <v>657.0</v>
@@ -8343,7 +8706,7 @@
     </row>
     <row r="645">
       <c r="A645" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B645" s="1">
         <v>658.0</v>
@@ -8351,7 +8714,7 @@
     </row>
     <row r="646">
       <c r="A646" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B646" s="1">
         <v>659.0</v>
@@ -8359,23 +8722,20 @@
     </row>
     <row r="647">
       <c r="A647" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B647" s="1">
         <v>660.0</v>
       </c>
     </row>
     <row r="648">
-      <c r="A648" s="1" t="s">
-        <v>647</v>
-      </c>
       <c r="B648" s="1">
         <v>661.0</v>
       </c>
     </row>
     <row r="649">
       <c r="A649" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="B649" s="1">
         <v>662.0</v>
@@ -8383,7 +8743,7 @@
     </row>
     <row r="650">
       <c r="A650" s="1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="B650" s="1">
         <v>663.0</v>
@@ -8391,7 +8751,7 @@
     </row>
     <row r="651">
       <c r="A651" s="1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="B651" s="1">
         <v>664.0</v>
@@ -9797,332 +10157,332 @@
     </row>
     <row r="277">
       <c r="A277" s="1" t="s">
-        <v>500</v>
+        <v>648</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -10860,277 +11220,277 @@
     </row>
     <row r="144">
       <c r="A144" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>
@@ -11884,172 +12244,172 @@
     </row>
     <row r="147">
       <c r="A147" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
   </sheetData>
@@ -12597,157 +12957,157 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="s">
-        <v>616</v>
+        <v>650</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>
@@ -15971,4 +16331,1119 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="s">
+        <v>752</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>754</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>760</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="8" t="s">
+        <v>768</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="s">
+        <v>770</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="s">
+        <v>771</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="s">
+        <v>772</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="s">
+        <v>774</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="s">
+        <v>776</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="s">
+        <v>777</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="9" t="s">
+        <v>778</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="s">
+        <v>779</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="s">
+        <v>780</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="s">
+        <v>781</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="s">
+        <v>783</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="s">
+        <v>785</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="9" t="s">
+        <v>786</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="9" t="s">
+        <v>788</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="9" t="s">
+        <v>790</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="9" t="s">
+        <v>792</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="9" t="s">
+        <v>795</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="9" t="s">
+        <v>799</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="9" t="s">
+        <v>801</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="5" t="s">
+        <v>812</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="9" t="s">
+        <v>813</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="9" t="s">
+        <v>815</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="9" t="s">
+        <v>817</v>
+      </c>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="5" t="s">
+        <v>818</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="10" t="s">
+        <v>819</v>
+      </c>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="10" t="s">
+        <v>821</v>
+      </c>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="10" t="s">
+        <v>822</v>
+      </c>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="11" t="s">
+        <v>823</v>
+      </c>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="10" t="s">
+        <v>824</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="10" t="s">
+        <v>825</v>
+      </c>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="10" t="s">
+        <v>826</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="10" t="s">
+        <v>827</v>
+      </c>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="10" t="s">
+        <v>829</v>
+      </c>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="10" t="s">
+        <v>830</v>
+      </c>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="10" t="s">
+        <v>837</v>
+      </c>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="10" t="s">
+        <v>840</v>
+      </c>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="10" t="s">
+        <v>841</v>
+      </c>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="10" t="s">
+        <v>842</v>
+      </c>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="10" t="s">
+        <v>843</v>
+      </c>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="10" t="s">
+        <v>844</v>
+      </c>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="10" t="s">
+        <v>845</v>
+      </c>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="10" t="s">
+        <v>846</v>
+      </c>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="8" t="s">
+        <v>847</v>
+      </c>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="8" t="s">
+        <v>848</v>
+      </c>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="8" t="s">
+        <v>849</v>
+      </c>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>